<commit_message>
update lagi setelah sekian lama
</commit_message>
<xml_diff>
--- a/public/DataPegawai/Latihan.xlsx
+++ b/public/DataPegawai/Latihan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D083548-19BF-4064-87E5-DC88D7C5022E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34492F7-36D1-4B58-93BE-803502431E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C42593F4-95A7-403E-A2D7-1B57A1432229}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C42593F4-95A7-403E-A2D7-1B57A1432229}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Abraham</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Barabai</t>
   </si>
   <si>
-    <t>Sutrisno</t>
-  </si>
-  <si>
     <t>Kandangan</t>
+  </si>
+  <si>
+    <t>Banjarmasin</t>
+  </si>
+  <si>
+    <t>Tabalong</t>
+  </si>
+  <si>
+    <t>Jokowi</t>
+  </si>
+  <si>
+    <t>Prabowo</t>
+  </si>
+  <si>
+    <t>Gibran</t>
+  </si>
+  <si>
+    <t>Ganjar</t>
   </si>
 </sst>
 </file>
@@ -397,33 +409,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25AE246-B29B-4006-9EEF-2C1A6F768280}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>20202</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>76767</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>99002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>85621</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>